<commit_message>
save excel data into db
</commit_message>
<xml_diff>
--- a/src/main/java/cz/kct/testApp.xlsx
+++ b/src/main/java/cz/kct/testApp.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artem.belyshev\IdeaProjects\kct.data.spring\src\main\java\cz\kct\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2ACAB9C1-175A-4987-B977-FD1872FB2EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44436C58-51C2-4A2B-A447-2E74A8C5B10F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2385" yWindow="480" windowWidth="19575" windowHeight="14295" xr2:uid="{62FA5389-0F21-4141-8491-0A27E1030148}"/>
+    <workbookView xWindow="2385" yWindow="480" windowWidth="19575" windowHeight="14295" activeTab="2" xr2:uid="{62FA5389-0F21-4141-8491-0A27E1030148}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
-    <sheet name="My Sec ExcelSheet" r:id="rId5" sheetId="2"/>
-    <sheet name="Test table" r:id="rId6" sheetId="3"/>
+    <sheet name="My Sec ExcelSheet" sheetId="2" r:id="rId2"/>
+    <sheet name="Test table" sheetId="3" r:id="rId3"/>
+    <sheet name="Values" r:id="rId7" sheetId="4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>SNo</t>
   </si>
@@ -119,7 +120,7 @@
     <t>value</t>
   </si>
   <si>
-    <t>10</t>
+    <t>16</t>
   </si>
 </sst>
 </file>
@@ -156,8 +157,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -474,7 +478,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E283450E-971D-4B84-BC5E-D1A2B46DD728}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -483,14 +487,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
@@ -504,7 +508,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s" s="0">
         <v>4</v>
       </c>
@@ -518,7 +522,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s" s="0">
         <v>8</v>
       </c>
@@ -532,7 +536,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s" s="0">
         <v>12</v>
       </c>
@@ -546,7 +550,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s" s="0">
         <v>16</v>
       </c>
@@ -560,7 +564,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s" s="0">
         <v>20</v>
       </c>
@@ -574,7 +578,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s" s="0">
         <v>24</v>
       </c>
@@ -589,11 +593,42 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:B2"/>
   <sheetViews>

</xml_diff>